<commit_message>
modified data dictionary and adding DDL for database
</commit_message>
<xml_diff>
--- a/watching_data_dictionary.xlsx
+++ b/watching_data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Watching\Watching\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4E8AECB-4B63-4748-9196-306D457586AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADD058F-7A52-4638-8920-C86D50918A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45525" yWindow="2760" windowWidth="22215" windowHeight="11490" xr2:uid="{3D911F35-36B8-4F4B-8FCC-BD2553436341}"/>
+    <workbookView xWindow="44805" yWindow="1650" windowWidth="22215" windowHeight="11490" xr2:uid="{3D911F35-36B8-4F4B-8FCC-BD2553436341}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="149">
   <si>
     <t>Column name in file</t>
   </si>
@@ -521,6 +521,9 @@
   </si>
   <si>
     <t>Very Prestigious</t>
+  </si>
+  <si>
+    <t>wr_category</t>
   </si>
 </sst>
 </file>
@@ -556,12 +559,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3371EFA7-AEC8-4E4E-A6B2-0F7AEB05F79C}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1064,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>148</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>
@@ -1415,7 +1417,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>94</v>
       </c>
       <c r="B10" t="s">

</xml_diff>